<commit_message>
diverse collections figures and plots updates
</commit_message>
<xml_diff>
--- a/analyses/data/LocationData.xlsx
+++ b/analyses/data/LocationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lexikeene/Documents/Research/diverse_collections/R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lexikeene/Documents/Research/diverse_collections/github/analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5750B3A3-78EE-AF4B-89F8-08AEA2662253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF2A53D-45C9-F04E-95B7-9C06AF1A5CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="500" windowWidth="14700" windowHeight="15860" xr2:uid="{1D392CE1-C1B7-5B4F-A5CD-CD91EAEAFFF0}"/>
+    <workbookView xWindow="7420" yWindow="760" windowWidth="14700" windowHeight="15860" xr2:uid="{1D392CE1-C1B7-5B4F-A5CD-CD91EAEAFFF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>number</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>ME</t>
+  </si>
+  <si>
+    <t>JFK Parkway</t>
   </si>
 </sst>
 </file>
@@ -164,9 +167,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,7 +207,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -310,7 +313,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4201E3-4104-2747-B819-36548A90AB07}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,62 +620,76 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>541</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10">
-        <v>40.818320999999997</v>
+        <v>40.525444999999998</v>
       </c>
       <c r="E10">
-        <v>-81.932565999999994</v>
+        <v>-105.07343899999999</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>660</v>
+        <v>541</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11">
-        <v>40.822166000000003</v>
+        <v>40.818320999999997</v>
       </c>
       <c r="E11">
-        <v>-77.889156999999997</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>-81.932565999999994</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>660</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>40.822166000000003</v>
+      </c>
+      <c r="E12">
+        <v>-77.889156999999997</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>44.529775000000001</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>-69.630373000000006</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E16" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>